<commit_message>
Acréscimo lançamentos futuros jan_ago
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projeto_planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\projeto_planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>29/10</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>ANUIDADE DIFERENCIADA TIT-PARC 01/12 BR</t>
+  </si>
+  <si>
+    <t>Riachuelo</t>
+  </si>
+  <si>
+    <t>Atacado dos Presentes</t>
   </si>
 </sst>
 </file>
@@ -645,6 +651,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,7 +664,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -946,18 +952,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q121"/>
+  <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P89" sqref="P89"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" customWidth="1"/>
-    <col min="3" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2460,10 +2466,10 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="43"/>
+      <c r="B56" s="44"/>
       <c r="C56" s="22"/>
       <c r="D56" s="23"/>
       <c r="E56" s="23"/>
@@ -2939,10 +2945,10 @@
       <c r="O76" s="6"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A77" s="42" t="s">
+      <c r="A77" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B77" s="43"/>
+      <c r="B77" s="44"/>
       <c r="C77" s="22"/>
       <c r="D77" s="23"/>
       <c r="E77" s="23"/>
@@ -2964,10 +2970,10 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="42" t="s">
+      <c r="A78" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="43"/>
+      <c r="B78" s="44"/>
       <c r="C78" s="22"/>
       <c r="D78" s="23"/>
       <c r="E78" s="23"/>
@@ -2987,7 +2993,7 @@
         <f>SUM(N78)</f>
         <v>3906.8900000000003</v>
       </c>
-      <c r="Q78" s="44"/>
+      <c r="Q78" s="40"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="37"/>
@@ -3022,7 +3028,7 @@
       <c r="M80" s="37"/>
       <c r="N80" s="37"/>
       <c r="O80" s="37"/>
-      <c r="Q80" s="44"/>
+      <c r="Q80" s="40"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="26">
@@ -3873,125 +3879,161 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
-        <v>45988</v>
+        <v>46003</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="C109" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="D109" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="E109" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="F109" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="G109" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="H109" s="12">
-        <v>55.74</v>
-      </c>
+        <v>55.77</v>
+      </c>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
-      <c r="O109" s="9">
-        <f>SUM(C109:H109)</f>
-        <v>334.44</v>
+      <c r="O109" s="12">
+        <v>55.77</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B110" s="41"/>
-      <c r="C110" s="29">
-        <f t="shared" ref="C110:H110" si="0">SUM(C82:C109)</f>
-        <v>2228.9899999999998</v>
-      </c>
-      <c r="D110" s="29">
-        <f t="shared" si="0"/>
-        <v>1566.17</v>
-      </c>
-      <c r="E110" s="29">
-        <f t="shared" si="0"/>
-        <v>1116.3399999999999</v>
-      </c>
-      <c r="F110" s="29">
-        <f t="shared" si="0"/>
-        <v>895.82</v>
-      </c>
-      <c r="G110" s="29">
-        <f t="shared" si="0"/>
-        <v>730.24</v>
-      </c>
-      <c r="H110" s="29">
-        <f t="shared" si="0"/>
-        <v>317.99</v>
-      </c>
+      <c r="A110" s="7">
+        <v>46002</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C110" s="12">
+        <v>203.32</v>
+      </c>
+      <c r="D110" s="12">
+        <v>203.32</v>
+      </c>
+      <c r="E110" s="12">
+        <v>203.32</v>
+      </c>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
-      <c r="O110" s="29">
-        <f>SUM(C110:H110)</f>
-        <v>6855.5499999999993</v>
+      <c r="O110" s="9">
+        <v>609.96</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A111" s="37"/>
-      <c r="B111" s="37"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="37"/>
-      <c r="F111" s="37"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="37"/>
-      <c r="I111" s="37"/>
-      <c r="J111" s="37"/>
-      <c r="K111" s="37"/>
-      <c r="L111" s="37"/>
-      <c r="M111" s="37"/>
-      <c r="N111" s="37"/>
-      <c r="O111" s="37"/>
+      <c r="A111" s="7">
+        <v>45988</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="D111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="E111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="F111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="G111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="H111" s="12">
+        <v>55.74</v>
+      </c>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="9">
+        <f>SUM(C111:H111)</f>
+        <v>334.44</v>
+      </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="37"/>
-      <c r="B112" s="37"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="37"/>
-      <c r="G112" s="37"/>
-      <c r="H112" s="37"/>
-      <c r="I112" s="37"/>
-      <c r="J112" s="37"/>
-      <c r="K112" s="37"/>
-      <c r="L112" s="37"/>
-      <c r="M112" s="37"/>
-      <c r="N112" s="37"/>
-      <c r="O112" s="37"/>
+      <c r="A112" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" s="42"/>
+      <c r="C112" s="29">
+        <f>SUM(C82:C111)</f>
+        <v>2488.08</v>
+      </c>
+      <c r="D112" s="29">
+        <f>SUM(D82:D111)</f>
+        <v>1769.49</v>
+      </c>
+      <c r="E112" s="29">
+        <f>SUM(E82:E111)</f>
+        <v>1319.6599999999999</v>
+      </c>
+      <c r="F112" s="29">
+        <f>SUM(F82:F111)</f>
+        <v>895.82</v>
+      </c>
+      <c r="G112" s="29">
+        <f>SUM(G82:G111)</f>
+        <v>730.24</v>
+      </c>
+      <c r="H112" s="29">
+        <f>SUM(H82:H111)</f>
+        <v>317.99</v>
+      </c>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="29">
+        <f>SUM(C112:H112)</f>
+        <v>7521.2799999999988</v>
+      </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="37"/>
       <c r="B113" s="37"/>
-      <c r="C113" s="37"/>
-      <c r="D113" s="37"/>
-      <c r="E113" s="37"/>
-      <c r="F113" s="37"/>
-      <c r="G113" s="37"/>
-      <c r="H113" s="37"/>
-      <c r="I113" s="37"/>
-      <c r="J113" s="37"/>
+      <c r="C113" s="12">
+        <v>2396.9699999999998</v>
+      </c>
+      <c r="D113" s="12">
+        <v>2239.48</v>
+      </c>
+      <c r="E113" s="12">
+        <v>1596.54</v>
+      </c>
+      <c r="F113" s="12">
+        <v>1010.3</v>
+      </c>
+      <c r="G113" s="12">
+        <v>844.75</v>
+      </c>
+      <c r="H113" s="12">
+        <v>432.51</v>
+      </c>
+      <c r="I113" s="12">
+        <v>262.25</v>
+      </c>
+      <c r="J113" s="12">
+        <v>262.25</v>
+      </c>
       <c r="K113" s="37"/>
       <c r="L113" s="37"/>
       <c r="M113" s="37"/>
@@ -4134,9 +4176,43 @@
       <c r="N121" s="37"/>
       <c r="O121" s="37"/>
     </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" s="37"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="37"/>
+      <c r="J122" s="37"/>
+      <c r="K122" s="37"/>
+      <c r="L122" s="37"/>
+      <c r="M122" s="37"/>
+      <c r="N122" s="37"/>
+      <c r="O122" s="37"/>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" s="37"/>
+      <c r="B123" s="37"/>
+      <c r="C123" s="37"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="37"/>
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="37"/>
+      <c r="J123" s="37"/>
+      <c r="K123" s="37"/>
+      <c r="L123" s="37"/>
+      <c r="M123" s="37"/>
+      <c r="N123" s="37"/>
+      <c r="O123" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A112:B112"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>

</xml_diff>

<commit_message>
adicionando 11/25 e 01/26
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\projeto_planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\projeto_planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="155">
   <si>
     <t>29/10</t>
   </si>
@@ -314,12 +314,6 @@
     <t>ANUIDADE DIFERENCIADA TIT-PARC 01/12 BR</t>
   </si>
   <si>
-    <t>Riachuelo</t>
-  </si>
-  <si>
-    <t>Atacado dos Presentes</t>
-  </si>
-  <si>
     <t>BUSON PARC 06/06 SAO JOSE DOSBR</t>
   </si>
   <si>
@@ -384,6 +378,117 @@
   </si>
   <si>
     <t>Lançamento Futuro</t>
+  </si>
+  <si>
+    <t>ESTORNO ANUIDADE BR</t>
+  </si>
+  <si>
+    <t>Jose Ronierio Marinho Osasco BR</t>
+  </si>
+  <si>
+    <t>Compra / Vencimento 10/01</t>
+  </si>
+  <si>
+    <t>09/12</t>
+  </si>
+  <si>
+    <t>REST ENTRE AMIGOS RECIFE BR</t>
+  </si>
+  <si>
+    <t>02/12</t>
+  </si>
+  <si>
+    <t>NETFLIX.COM SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>18/12</t>
+  </si>
+  <si>
+    <t>AMAZON BR SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>19/12</t>
+  </si>
+  <si>
+    <t>AMAZONMKTPLC*PUCCIIMPO SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>21/12</t>
+  </si>
+  <si>
+    <t>20/12</t>
+  </si>
+  <si>
+    <t>IFD*SUPERMERCADO GAIVO RECIFE BR</t>
+  </si>
+  <si>
+    <t>22/12</t>
+  </si>
+  <si>
+    <t>03/12</t>
+  </si>
+  <si>
+    <t>UBER CASH SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>04/12</t>
+  </si>
+  <si>
+    <t>UBER * PENDING SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>11/12</t>
+  </si>
+  <si>
+    <t>DL *GOOGLE HBO Max Str SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>07/12</t>
+  </si>
+  <si>
+    <t>DL*GOOGLE Paramo SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>Amazon Prime Aluguel SAO PAULO BR</t>
+  </si>
+  <si>
+    <t>27/09</t>
+  </si>
+  <si>
+    <t>28/10</t>
+  </si>
+  <si>
+    <t>MLP*Magalu Sa PARC 02/04 BRAGANCA PAUBR</t>
+  </si>
+  <si>
+    <t>29/11</t>
+  </si>
+  <si>
+    <t>MERCADOLIVRE* PARC 01/03 FRANCA BR</t>
+  </si>
+  <si>
+    <t>06/12</t>
+  </si>
+  <si>
+    <t>10/12</t>
+  </si>
+  <si>
+    <t>SUPERMERCADO PARC 01/03 RECIFE BR</t>
+  </si>
+  <si>
+    <t>RIACHUELO-FIL PARC 01/03 RECIFE BR</t>
+  </si>
+  <si>
+    <t>12/12</t>
+  </si>
+  <si>
+    <t>ATACADO DOS P PARC 01/02 RECIFE BR</t>
+  </si>
+  <si>
+    <t>23/12</t>
+  </si>
+  <si>
+    <t>HNA PARC 01/10 RECIFE BR</t>
   </si>
 </sst>
 </file>
@@ -396,7 +501,7 @@
     <numFmt numFmtId="164" formatCode="d/m;@"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,8 +552,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +612,30 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="53"/>
       </patternFill>
     </fill>
   </fills>
@@ -613,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -739,11 +874,41 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1033,25 +1198,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q123"/>
+  <dimension ref="A1:Q158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
     <col min="3" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="29">
         <v>2025</v>
       </c>
@@ -1098,7 +1263,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>45971</v>
       </c>
@@ -1121,7 +1286,7 @@
       </c>
       <c r="O2" s="17"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="33">
         <v>45972</v>
       </c>
@@ -1144,7 +1309,7 @@
       </c>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="33">
         <v>45980</v>
       </c>
@@ -1167,7 +1332,7 @@
       </c>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>45834</v>
       </c>
@@ -1201,7 +1366,7 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>45959</v>
       </c>
@@ -1227,7 +1392,7 @@
         <v>22.86</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>45930</v>
       </c>
@@ -1255,7 +1420,7 @@
         <v>65.86</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1446,7 @@
         <v>52.81</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1472,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1502,7 @@
         <v>174.3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
@@ -1365,7 +1530,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1405,7 +1570,7 @@
         <v>1287.93</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>45964</v>
       </c>
@@ -1428,7 +1593,7 @@
       </c>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>45965</v>
       </c>
@@ -1453,7 +1618,7 @@
         <v>75.040000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>45965</v>
       </c>
@@ -1478,7 +1643,7 @@
         <v>121.26</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>45905</v>
       </c>
@@ -1503,7 +1668,7 @@
         <v>55.74</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>45905</v>
       </c>
@@ -1533,7 +1698,7 @@
         <v>215.96999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>45966</v>
       </c>
@@ -1558,7 +1723,7 @@
         <v>729.61</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>45966</v>
       </c>
@@ -1583,7 +1748,7 @@
         <v>723.79</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>45936</v>
       </c>
@@ -1611,7 +1776,7 @@
         <v>421.78</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>45876</v>
       </c>
@@ -1643,7 +1808,7 @@
         <v>335.52</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>45966</v>
       </c>
@@ -1666,7 +1831,7 @@
       </c>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>45966</v>
       </c>
@@ -1689,7 +1854,7 @@
       </c>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>45966</v>
       </c>
@@ -1712,7 +1877,7 @@
       </c>
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>45966</v>
       </c>
@@ -1735,7 +1900,7 @@
       </c>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>45966</v>
       </c>
@@ -1758,7 +1923,7 @@
       </c>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>45966</v>
       </c>
@@ -1781,7 +1946,7 @@
       </c>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>45966</v>
       </c>
@@ -1804,7 +1969,7 @@
       </c>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>45966</v>
       </c>
@@ -1827,7 +1992,7 @@
       </c>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>45908</v>
       </c>
@@ -1857,7 +2022,7 @@
         <v>89.19</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>45878</v>
       </c>
@@ -1889,7 +2054,7 @@
         <v>314.2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>45941</v>
       </c>
@@ -1914,7 +2079,7 @@
         <v>119.71</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>45942</v>
       </c>
@@ -1942,7 +2107,7 @@
         <v>124.86</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>45942</v>
       </c>
@@ -1970,7 +2135,7 @@
         <v>40.94</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>45701</v>
       </c>
@@ -2014,7 +2179,7 @@
         <v>1032.3999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>45702</v>
       </c>
@@ -2058,8 +2223,8 @@
         <v>1116.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
         <v>45915</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -2088,7 +2253,7 @@
         <v>391.26</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>45964</v>
       </c>
@@ -2111,7 +2276,7 @@
       </c>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>45964</v>
       </c>
@@ -2134,7 +2299,7 @@
       </c>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>45964</v>
       </c>
@@ -2157,7 +2322,7 @@
       </c>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>45964</v>
       </c>
@@ -2180,7 +2345,7 @@
       </c>
       <c r="O41" s="6"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>45964</v>
       </c>
@@ -2203,7 +2368,7 @@
       </c>
       <c r="O42" s="6"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>45858</v>
       </c>
@@ -2237,7 +2402,7 @@
         <v>299.95</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>45858</v>
       </c>
@@ -2271,7 +2436,7 @@
         <v>263.7</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>45923</v>
       </c>
@@ -2296,7 +2461,7 @@
         <v>290.99</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>45984</v>
       </c>
@@ -2321,7 +2486,7 @@
         <v>52.27</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>45984</v>
       </c>
@@ -2346,7 +2511,7 @@
         <v>75.28</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>45984</v>
       </c>
@@ -2371,7 +2536,7 @@
         <v>37.64</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>45954</v>
       </c>
@@ -2396,7 +2561,7 @@
         <v>96.66</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>45954</v>
       </c>
@@ -2421,7 +2586,7 @@
         <v>40.32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>45954</v>
       </c>
@@ -2446,7 +2611,7 @@
         <v>99.73</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>45954</v>
       </c>
@@ -2471,7 +2636,7 @@
         <v>162.52000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>45987</v>
       </c>
@@ -2496,7 +2661,7 @@
         <v>44.81</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>45987</v>
       </c>
@@ -2521,7 +2686,7 @@
         <v>31.06</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>45988</v>
       </c>
@@ -2546,7 +2711,7 @@
         <v>55.74</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="43" t="s">
         <v>86</v>
       </c>
@@ -2571,7 +2736,7 @@
         <v>2893.7400000000007</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="36"/>
       <c r="B57" s="36"/>
       <c r="C57" s="36"/>
@@ -2588,7 +2753,7 @@
       <c r="N57" s="36"/>
       <c r="O57" s="36"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="37" t="s">
         <v>66</v>
       </c>
@@ -2611,7 +2776,7 @@
       </c>
       <c r="O58" s="6"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>0</v>
       </c>
@@ -2634,7 +2799,7 @@
       </c>
       <c r="O59" s="6"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="37" t="s">
         <v>66</v>
       </c>
@@ -2657,7 +2822,7 @@
       </c>
       <c r="O60" s="6"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="37" t="s">
         <v>3</v>
       </c>
@@ -2680,7 +2845,7 @@
       </c>
       <c r="O61" s="6"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="37" t="s">
         <v>67</v>
       </c>
@@ -2703,7 +2868,7 @@
       </c>
       <c r="O62" s="6"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="37" t="s">
         <v>68</v>
       </c>
@@ -2726,7 +2891,7 @@
       </c>
       <c r="O63" s="6"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="37" t="s">
         <v>68</v>
       </c>
@@ -2749,7 +2914,7 @@
       </c>
       <c r="O64" s="6"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="37" t="s">
         <v>68</v>
       </c>
@@ -2772,7 +2937,7 @@
       </c>
       <c r="O65" s="6"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="37" t="s">
         <v>69</v>
       </c>
@@ -2795,7 +2960,7 @@
       </c>
       <c r="O66" s="6"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="37" t="s">
         <v>69</v>
       </c>
@@ -2818,7 +2983,7 @@
       </c>
       <c r="O67" s="6"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="37" t="s">
         <v>69</v>
       </c>
@@ -2841,7 +3006,7 @@
       </c>
       <c r="O68" s="6"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="37" t="s">
         <v>70</v>
       </c>
@@ -2864,7 +3029,7 @@
       </c>
       <c r="O69" s="6"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="37" t="s">
         <v>71</v>
       </c>
@@ -2887,7 +3052,7 @@
       </c>
       <c r="O70" s="6"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="37" t="s">
         <v>72</v>
       </c>
@@ -2910,7 +3075,7 @@
       </c>
       <c r="O71" s="6"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="37" t="s">
         <v>73</v>
       </c>
@@ -2933,7 +3098,7 @@
       </c>
       <c r="O72" s="6"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="37" t="s">
         <v>90</v>
       </c>
@@ -2956,7 +3121,7 @@
       </c>
       <c r="O73" s="6"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="37" t="s">
         <v>94</v>
       </c>
@@ -2979,7 +3144,7 @@
       </c>
       <c r="O74" s="6"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="37" t="s">
         <v>68</v>
       </c>
@@ -3002,7 +3167,7 @@
       </c>
       <c r="O75" s="6"/>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="37" t="s">
         <v>93</v>
       </c>
@@ -3025,7 +3190,7 @@
       </c>
       <c r="O76" s="6"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="43" t="s">
         <v>87</v>
       </c>
@@ -3050,7 +3215,7 @@
         <v>1013.1499999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="43" t="s">
         <v>88</v>
       </c>
@@ -3076,7 +3241,7 @@
       </c>
       <c r="Q78" s="39"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="36"/>
       <c r="B79" s="36"/>
       <c r="C79" s="36"/>
@@ -3093,7 +3258,7 @@
       <c r="N79" s="36"/>
       <c r="O79" s="36"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="36"/>
       <c r="B80" s="36"/>
       <c r="C80" s="36"/>
@@ -3111,12 +3276,12 @@
       <c r="O80" s="36"/>
       <c r="Q80" s="39"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="26">
         <v>2026</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>9</v>
@@ -3158,51 +3323,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="7">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82" s="47">
+        <v>46358</v>
+      </c>
+      <c r="B82" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="2">
+        <v>-45.5</v>
+      </c>
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="48"/>
+      <c r="I82" s="48"/>
+      <c r="J82" s="48"/>
+      <c r="K82" s="48"/>
+      <c r="L82" s="48"/>
+      <c r="M82" s="48"/>
+      <c r="N82" s="48"/>
+      <c r="O82" s="17"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A83" s="7">
         <v>45834</v>
       </c>
-      <c r="B82" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C82" s="9">
+      <c r="B83" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="9">
         <v>54.5</v>
       </c>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4"/>
-      <c r="O82" s="9">
-        <f>SUM(C82)</f>
-        <v>54.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="7">
-        <v>45959</v>
-      </c>
-      <c r="B83" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83" s="9">
-        <v>22.86</v>
-      </c>
-      <c r="D83" s="9">
-        <v>22.86</v>
-      </c>
-      <c r="E83" s="9">
-        <v>22.86</v>
-      </c>
-      <c r="F83" s="9">
-        <v>22.86</v>
-      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
@@ -3211,24 +3367,22 @@
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
-      <c r="O83" s="12">
-        <f>SUM(C83:N83)</f>
-        <v>91.44</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
-        <v>45930</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C84" s="9">
-        <v>32.93</v>
-      </c>
-      <c r="D84" s="9">
-        <v>32.93</v>
-      </c>
+      <c r="O83" s="9">
+        <f>SUM(C83)</f>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A84" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B84" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="53">
+        <v>34.090000000000003</v>
+      </c>
+      <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -3239,27 +3393,22 @@
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
       <c r="N84" s="4"/>
-      <c r="O84" s="5">
-        <f>SUM(C84:D84)</f>
-        <v>65.86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="9">
-        <v>52.81</v>
-      </c>
-      <c r="D85" s="9">
-        <v>52.81</v>
-      </c>
-      <c r="E85" s="9">
-        <v>52.81</v>
-      </c>
+      <c r="O84" s="9"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="53">
+        <v>165.26</v>
+      </c>
+      <c r="D85" s="53">
+        <v>165.26</v>
+      </c>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -3269,30 +3418,23 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
-      <c r="O85" s="12">
-        <f>SUM(C85,D85,E85)</f>
-        <v>158.43</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C86" s="9">
-        <v>29.8</v>
-      </c>
-      <c r="D86" s="9">
-        <v>29.8</v>
-      </c>
-      <c r="E86" s="9">
-        <v>29.8</v>
-      </c>
-      <c r="F86" s="9">
-        <v>29.8</v>
-      </c>
+      <c r="O85" s="9"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C86" s="53">
+        <v>29.58</v>
+      </c>
+      <c r="D86" s="53">
+        <v>29.58</v>
+      </c>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -3301,28 +3443,27 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
-      <c r="O86" s="12">
-        <f>SUM(C86:F86)</f>
-        <v>119.2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" s="28" t="s">
-        <v>46</v>
+      <c r="O86" s="9"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="7">
+        <v>45959</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="C87" s="9">
-        <v>58.1</v>
+        <v>22.86</v>
       </c>
       <c r="D87" s="9">
-        <v>58.1</v>
+        <v>22.86</v>
       </c>
       <c r="E87" s="9">
-        <v>58.1</v>
-      </c>
-      <c r="F87" s="4"/>
+        <v>22.86</v>
+      </c>
+      <c r="F87" s="9">
+        <v>22.86</v>
+      </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -3333,23 +3474,25 @@
       <c r="N87" s="4"/>
       <c r="O87" s="12">
         <f>SUM(C87:N87)</f>
-        <v>174.3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="C88" s="9">
-        <v>183.99</v>
-      </c>
-      <c r="D88" s="9">
-        <v>183.99</v>
-      </c>
-      <c r="E88" s="4"/>
+        <v>91.44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="C88" s="56">
+        <v>21.63</v>
+      </c>
+      <c r="D88" s="56">
+        <v>21.63</v>
+      </c>
+      <c r="E88" s="56">
+        <v>21.63</v>
+      </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -3359,25 +3502,24 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
-      <c r="O88" s="12">
-        <f>SUM(C88,D88)</f>
-        <v>367.98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="7">
-        <v>45965</v>
+      <c r="O88" s="12"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C89" s="12">
-        <v>75.040000000000006</v>
-      </c>
-      <c r="D89" s="12">
-        <v>75.040000000000006</v>
-      </c>
-      <c r="E89" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="C89" s="9">
+        <v>52.81</v>
+      </c>
+      <c r="D89" s="9">
+        <v>52.81</v>
+      </c>
+      <c r="E89" s="9">
+        <v>52.81</v>
+      </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -3387,33 +3529,31 @@
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
-      <c r="O89" s="9">
-        <f>SUM(C89:N89)</f>
-        <v>150.08000000000001</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="7">
-        <v>45965</v>
+      <c r="O89" s="12">
+        <f>SUM(C89,D89,E89)</f>
+        <v>158.43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C90" s="12">
-        <v>121.26</v>
-      </c>
-      <c r="D90" s="12">
-        <v>121.26</v>
-      </c>
-      <c r="E90" s="12">
-        <v>121.26</v>
-      </c>
-      <c r="F90" s="12">
-        <v>121.26</v>
-      </c>
-      <c r="G90" s="12">
-        <v>121.26</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C90" s="9">
+        <v>29.8</v>
+      </c>
+      <c r="D90" s="9">
+        <v>29.8</v>
+      </c>
+      <c r="E90" s="9">
+        <v>29.8</v>
+      </c>
+      <c r="F90" s="9">
+        <v>29.8</v>
+      </c>
+      <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
@@ -3421,22 +3561,24 @@
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
-      <c r="O90" s="9">
-        <f>SUM(C90:G90)</f>
-        <v>606.30000000000007</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O90" s="12">
+        <f>SUM(C90:F90)</f>
+        <v>119.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
-        <v>45905</v>
-      </c>
-      <c r="B91" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C91" s="12">
-        <v>71.989999999999995</v>
-      </c>
-      <c r="D91" s="4"/>
+        <v>45930</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="9">
+        <v>32.93</v>
+      </c>
+      <c r="D91" s="9">
+        <v>32.93</v>
+      </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
@@ -3447,23 +3589,27 @@
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
-      <c r="O91" s="9">
-        <f>SUM(C91)</f>
-        <v>71.989999999999995</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="7">
-        <v>45936</v>
+      <c r="O91" s="5">
+        <f>SUM(C91:D91)</f>
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C92" s="12">
-        <v>210.89</v>
-      </c>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="C92" s="9">
+        <v>58.09</v>
+      </c>
+      <c r="D92" s="9">
+        <v>58.09</v>
+      </c>
+      <c r="E92" s="9">
+        <v>58.09</v>
+      </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
@@ -3473,22 +3619,24 @@
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
-      <c r="O92" s="9">
-        <f>SUM(C92)</f>
-        <v>210.89</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="7">
-        <v>45876</v>
+      <c r="O92" s="12">
+        <f>SUM(C92:N92)</f>
+        <v>174.27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C93" s="12">
-        <v>83.88</v>
-      </c>
-      <c r="D93" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="C93" s="9">
+        <v>183.99</v>
+      </c>
+      <c r="D93" s="9">
+        <v>183.99</v>
+      </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
@@ -3499,22 +3647,24 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
-      <c r="O93" s="9">
-        <f>SUM(C93)</f>
-        <v>83.88</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O93" s="12">
+        <f>SUM(C93,D93)</f>
+        <v>367.98</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
-        <v>45908</v>
+        <v>45965</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="C94" s="12">
-        <v>29.73</v>
-      </c>
-      <c r="D94" s="4"/>
+        <v>75.040000000000006</v>
+      </c>
+      <c r="D94" s="12">
+        <v>75.040000000000006</v>
+      </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -3526,28 +3676,32 @@
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
       <c r="O94" s="9">
-        <f>SUM(C94)</f>
-        <v>29.73</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C94:N94)</f>
+        <v>150.08000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
-        <v>45878</v>
+        <v>45965</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C95" s="12">
-        <v>78.55</v>
+        <v>121.25</v>
       </c>
       <c r="D95" s="12">
-        <v>78.55</v>
+        <v>121.25</v>
       </c>
       <c r="E95" s="12">
-        <v>78.55</v>
-      </c>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
+        <v>121.25</v>
+      </c>
+      <c r="F95" s="12">
+        <v>121.25</v>
+      </c>
+      <c r="G95" s="12">
+        <v>121.25</v>
+      </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
@@ -3556,19 +3710,19 @@
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="9">
-        <f>SUM(C95:E95)</f>
-        <v>235.64999999999998</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C95:G95)</f>
+        <v>606.25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
-        <v>45942</v>
+        <v>45905</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C96" s="12">
-        <v>62.43</v>
+        <v>71.989999999999995</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -3583,26 +3737,34 @@
       <c r="N96" s="4"/>
       <c r="O96" s="9">
         <f>SUM(C96)</f>
-        <v>62.43</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
-        <v>45942</v>
-      </c>
-      <c r="B97" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C97" s="12">
-        <v>20.47</v>
-      </c>
-      <c r="D97" s="12">
-        <v>20.47</v>
-      </c>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
+        <v>71.989999999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B97" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C97" s="56">
+        <v>114.59</v>
+      </c>
+      <c r="D97" s="56">
+        <v>114.59</v>
+      </c>
+      <c r="E97" s="56">
+        <v>114.59</v>
+      </c>
+      <c r="F97" s="56">
+        <v>114.59</v>
+      </c>
+      <c r="G97" s="56">
+        <v>114.59</v>
+      </c>
+      <c r="H97" s="56">
+        <v>114.59</v>
+      </c>
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
@@ -3610,19 +3772,19 @@
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
       <c r="O97" s="9">
-        <f>SUM(C97,D97)</f>
-        <v>40.94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C97)</f>
+        <v>114.59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
-        <v>45858</v>
+        <v>45936</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C98" s="12">
-        <v>52.74</v>
+        <v>210.89</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -3637,31 +3799,23 @@
       <c r="N98" s="4"/>
       <c r="O98" s="9">
         <f>SUM(C98)</f>
-        <v>52.74</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+        <v>210.89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="7">
-        <v>45923</v>
+        <v>45876</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C99" s="12">
-        <v>290.99</v>
-      </c>
-      <c r="D99" s="12">
-        <v>290.99</v>
-      </c>
-      <c r="E99" s="12">
-        <v>290.99</v>
-      </c>
-      <c r="F99" s="12">
-        <v>290.99</v>
-      </c>
-      <c r="G99" s="12">
-        <v>290.99</v>
-      </c>
+        <v>83.88</v>
+      </c>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
@@ -3670,23 +3824,21 @@
       <c r="M99" s="4"/>
       <c r="N99" s="4"/>
       <c r="O99" s="9">
-        <f>SUM(C99:G99)</f>
-        <v>1454.95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C99)</f>
+        <v>83.88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="7">
-        <v>45984</v>
+        <v>45908</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="C100" s="12">
-        <v>52.27</v>
-      </c>
-      <c r="D100" s="12">
-        <v>52.27</v>
-      </c>
+        <v>29.73</v>
+      </c>
+      <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
@@ -3698,29 +3850,27 @@
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
       <c r="O100" s="9">
-        <f>SUM(C100,D100)</f>
-        <v>104.54</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C100)</f>
+        <v>29.73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
-        <v>45984</v>
+        <v>45878</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C101" s="12">
-        <v>75.28</v>
+        <v>78.55</v>
       </c>
       <c r="D101" s="12">
-        <v>75.28</v>
+        <v>78.55</v>
       </c>
       <c r="E101" s="12">
-        <v>75.28</v>
-      </c>
-      <c r="F101" s="12">
-        <v>75.28</v>
-      </c>
+        <v>78.55</v>
+      </c>
+      <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -3730,29 +3880,27 @@
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
       <c r="O101" s="9">
-        <f>SUM(C101:F101)</f>
-        <v>301.12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" s="7">
-        <v>45984</v>
-      </c>
-      <c r="B102" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C102" s="12">
-        <v>37.64</v>
-      </c>
-      <c r="D102" s="12">
-        <v>37.64</v>
-      </c>
-      <c r="E102" s="12">
-        <v>37.64</v>
-      </c>
-      <c r="F102" s="12">
-        <v>37.64</v>
-      </c>
+        <f>SUM(C101:E101)</f>
+        <v>235.64999999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A102" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="B102" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C102" s="56">
+        <v>111.2</v>
+      </c>
+      <c r="D102" s="56">
+        <v>111.2</v>
+      </c>
+      <c r="E102" s="56">
+        <v>111.2</v>
+      </c>
+      <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
@@ -3761,23 +3909,24 @@
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
-      <c r="O102" s="9">
-        <f>SUM(C102:F102)</f>
-        <v>150.56</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103" s="7">
-        <v>45954</v>
-      </c>
-      <c r="B103" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C103" s="12">
-        <v>96.66</v>
-      </c>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
+      <c r="O102" s="9"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A103" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B103" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C103" s="56">
+        <v>203.32</v>
+      </c>
+      <c r="D103" s="56">
+        <v>203.32</v>
+      </c>
+      <c r="E103" s="56">
+        <v>203.32</v>
+      </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -3787,24 +3936,19 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
-      <c r="O103" s="9">
-        <f>SUM(C103)</f>
-        <v>96.66</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O103" s="9"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
-        <v>45954</v>
+        <v>45942</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="C104" s="12">
-        <v>40.32</v>
-      </c>
-      <c r="D104" s="12">
-        <v>40.32</v>
-      </c>
+        <v>62.43</v>
+      </c>
+      <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
@@ -3816,103 +3960,74 @@
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="9">
-        <f>SUM(C104,D104)</f>
-        <v>80.64</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C104)</f>
+        <v>62.43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
-        <v>45954</v>
+        <v>45942</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C105" s="12">
-        <v>99.73</v>
+        <v>20.47</v>
       </c>
       <c r="D105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="E105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="F105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="G105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="H105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="I105" s="12">
-        <v>99.73</v>
-      </c>
-      <c r="J105" s="12">
-        <v>99.73</v>
-      </c>
+        <v>20.47</v>
+      </c>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
       <c r="O105" s="9">
-        <f>SUM(C105:J105)</f>
-        <v>797.84</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" s="7">
-        <v>45954</v>
-      </c>
-      <c r="B106" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="D106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="E106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="F106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="G106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="H106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="I106" s="12">
-        <v>162.52000000000001</v>
-      </c>
-      <c r="J106" s="12">
-        <v>162.52000000000001</v>
-      </c>
+        <f>SUM(C105,D105)</f>
+        <v>40.94</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A106" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="B106" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C106" s="56">
+        <v>27.89</v>
+      </c>
+      <c r="D106" s="56">
+        <v>27.89</v>
+      </c>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
-      <c r="O106" s="9">
-        <f>SUM(C106:J106)</f>
-        <v>1300.1600000000001</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O106" s="9"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
-        <v>45987</v>
+        <v>45858</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="C107" s="12">
-        <v>44.81</v>
-      </c>
-      <c r="D107" s="12">
-        <v>44.81</v>
-      </c>
+        <v>52.74</v>
+      </c>
+      <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
@@ -3924,28 +4039,32 @@
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
       <c r="O107" s="9">
-        <f>SUM(C107:D107)</f>
-        <v>89.62</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C107)</f>
+        <v>52.74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="7">
-        <v>45987</v>
+        <v>45923</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C108" s="12">
-        <v>31.06</v>
+        <v>290.99</v>
       </c>
       <c r="D108" s="12">
-        <v>31.06</v>
+        <v>290.99</v>
       </c>
       <c r="E108" s="12">
-        <v>31.06</v>
-      </c>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
+        <v>290.99</v>
+      </c>
+      <c r="F108" s="12">
+        <v>290.99</v>
+      </c>
+      <c r="G108" s="12">
+        <v>290.99</v>
+      </c>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
@@ -3954,21 +4073,23 @@
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
       <c r="O108" s="9">
-        <f>SUM(C108:E108)</f>
-        <v>93.179999999999993</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+        <f>SUM(C108:G108)</f>
+        <v>1454.95</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="7">
-        <v>46003</v>
+        <v>45984</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="C109" s="12">
-        <v>55.77</v>
-      </c>
-      <c r="D109" s="4"/>
+        <v>52.25</v>
+      </c>
+      <c r="D109" s="12">
+        <v>52.25</v>
+      </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -3979,64 +4100,32 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
-      <c r="O109" s="12">
-        <v>55.77</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="7">
-        <v>46002</v>
-      </c>
-      <c r="B110" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C110" s="12">
-        <v>203.32</v>
-      </c>
-      <c r="D110" s="12">
-        <v>203.32</v>
-      </c>
-      <c r="E110" s="12">
-        <v>203.32</v>
-      </c>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="9">
-        <v>609.96</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O109" s="9">
+        <f>SUM(C109,D109)</f>
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="7">
-        <v>45988</v>
+        <v>45984</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C111" s="12">
-        <v>55.74</v>
+        <v>37.630000000000003</v>
       </c>
       <c r="D111" s="12">
-        <v>55.74</v>
+        <v>37.64</v>
       </c>
       <c r="E111" s="12">
-        <v>55.74</v>
+        <v>37.64</v>
       </c>
       <c r="F111" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="G111" s="12">
-        <v>55.74</v>
-      </c>
-      <c r="H111" s="12">
-        <v>55.74</v>
-      </c>
+        <v>37.64</v>
+      </c>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
@@ -4044,242 +4133,379 @@
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
       <c r="O111" s="9">
-        <f>SUM(C111:H111)</f>
-        <v>334.44</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="B112" s="42"/>
+        <f>SUM(C111:F111)</f>
+        <v>150.55000000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A112" s="7">
+        <v>45984</v>
+      </c>
+      <c r="B112" s="28" t="s">
+        <v>111</v>
+      </c>
       <c r="C112" s="12">
-        <f>SUM(C82:C111)</f>
-        <v>2488.08</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="D112" s="12">
-        <f t="shared" ref="D112:H112" si="0">SUM(D82:D111)</f>
-        <v>1769.49</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="E112" s="12">
-        <f t="shared" si="0"/>
-        <v>1319.6599999999999</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="F112" s="12">
-        <f t="shared" si="0"/>
-        <v>895.82</v>
-      </c>
-      <c r="G112" s="12">
-        <f t="shared" si="0"/>
-        <v>730.24</v>
-      </c>
-      <c r="H112" s="12">
-        <f t="shared" si="0"/>
-        <v>317.99</v>
-      </c>
+        <v>75.260000000000005</v>
+      </c>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
-      <c r="O112" s="12">
-        <f>SUM(C112:H112)</f>
-        <v>7521.2799999999988</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="B113" s="45"/>
-      <c r="C113" s="46">
-        <v>3277.31</v>
-      </c>
-      <c r="D113" s="12">
-        <v>2239.48</v>
-      </c>
-      <c r="E113" s="12">
-        <v>1596.54</v>
-      </c>
-      <c r="F113" s="12">
-        <v>1010.3</v>
-      </c>
-      <c r="G113" s="12">
-        <v>844.75</v>
-      </c>
-      <c r="H113" s="12">
-        <v>432.51</v>
-      </c>
-      <c r="I113" s="12">
-        <v>262.25</v>
-      </c>
-      <c r="J113" s="12">
-        <v>262.25</v>
-      </c>
+      <c r="O112" s="9">
+        <f>SUM(C112:F112)</f>
+        <v>301.04000000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A113" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B113" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C113" s="56">
+        <v>83.06</v>
+      </c>
+      <c r="D113" s="56">
+        <v>83.06</v>
+      </c>
+      <c r="E113" s="56">
+        <v>83.06</v>
+      </c>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
-      <c r="O113" s="40">
-        <f>SUM(C113:N113)</f>
-        <v>9925.3900000000012</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="36"/>
-      <c r="B114" s="36"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="36"/>
-      <c r="I114" s="36"/>
-      <c r="J114" s="36"/>
-      <c r="K114" s="36"/>
-      <c r="L114" s="36"/>
-      <c r="M114" s="36"/>
-      <c r="N114" s="36"/>
-      <c r="O114" s="36"/>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A115" s="36"/>
-      <c r="B115" s="36"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="36"/>
-      <c r="I115" s="36"/>
-      <c r="J115" s="36"/>
-      <c r="K115" s="36"/>
-      <c r="L115" s="36"/>
-      <c r="M115" s="36"/>
-      <c r="N115" s="36"/>
-      <c r="O115" s="36"/>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="36"/>
-      <c r="B116" s="36"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="36"/>
-      <c r="E116" s="36"/>
-      <c r="F116" s="36"/>
-      <c r="G116" s="36"/>
-      <c r="H116" s="36"/>
-      <c r="I116" s="36"/>
-      <c r="J116" s="36"/>
-      <c r="K116" s="36"/>
-      <c r="L116" s="36"/>
-      <c r="M116" s="36"/>
-      <c r="N116" s="36"/>
-      <c r="O116" s="36"/>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" s="36"/>
-      <c r="B117" s="36"/>
-      <c r="C117" s="36"/>
-      <c r="D117" s="36"/>
-      <c r="E117" s="36"/>
-      <c r="F117" s="36"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="36"/>
-      <c r="I117" s="36"/>
-      <c r="J117" s="36"/>
-      <c r="K117" s="36"/>
-      <c r="L117" s="36"/>
-      <c r="M117" s="36"/>
-      <c r="N117" s="36"/>
-      <c r="O117" s="36"/>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="36"/>
-      <c r="B118" s="36"/>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="36"/>
-      <c r="K118" s="36"/>
-      <c r="L118" s="36"/>
-      <c r="M118" s="36"/>
-      <c r="N118" s="36"/>
-      <c r="O118" s="36"/>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A119" s="36"/>
-      <c r="B119" s="36"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="36"/>
-      <c r="E119" s="36"/>
-      <c r="F119" s="36"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="36"/>
-      <c r="I119" s="36"/>
-      <c r="J119" s="36"/>
-      <c r="K119" s="36"/>
-      <c r="L119" s="36"/>
-      <c r="M119" s="36"/>
-      <c r="N119" s="36"/>
-      <c r="O119" s="36"/>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A120" s="36"/>
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
-      <c r="E120" s="36"/>
-      <c r="F120" s="36"/>
-      <c r="G120" s="36"/>
-      <c r="H120" s="36"/>
-      <c r="I120" s="36"/>
-      <c r="J120" s="36"/>
-      <c r="K120" s="36"/>
-      <c r="L120" s="36"/>
-      <c r="M120" s="36"/>
-      <c r="N120" s="36"/>
-      <c r="O120" s="36"/>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A121" s="36"/>
-      <c r="B121" s="36"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="36"/>
-      <c r="E121" s="36"/>
-      <c r="F121" s="36"/>
-      <c r="G121" s="36"/>
-      <c r="H121" s="36"/>
-      <c r="I121" s="36"/>
-      <c r="J121" s="36"/>
-      <c r="K121" s="36"/>
-      <c r="L121" s="36"/>
-      <c r="M121" s="36"/>
-      <c r="N121" s="36"/>
-      <c r="O121" s="36"/>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A122" s="36"/>
-      <c r="B122" s="36"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
-      <c r="F122" s="36"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="36"/>
-      <c r="I122" s="36"/>
-      <c r="J122" s="36"/>
-      <c r="K122" s="36"/>
-      <c r="L122" s="36"/>
-      <c r="M122" s="36"/>
-      <c r="N122" s="36"/>
-      <c r="O122" s="36"/>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O113" s="9"/>
+    </row>
+    <row r="114" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B114" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C114" s="12">
+        <v>96.66</v>
+      </c>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="9">
+        <f>SUM(C114)</f>
+        <v>96.66</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A115" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B115" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="D115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="E115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="F115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="G115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="H115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="I115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="J115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="K115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="L115" s="56">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="9"/>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A116" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C116" s="12">
+        <v>40.32</v>
+      </c>
+      <c r="D116" s="12">
+        <v>40.32</v>
+      </c>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="9">
+        <f>SUM(C116,D116)</f>
+        <v>80.64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A117" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="D117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="E117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="F117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="G117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="H117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="I117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="J117" s="12">
+        <v>99.73</v>
+      </c>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="9">
+        <f>SUM(C117:J117)</f>
+        <v>797.84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A118" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="D118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="E118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="F118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="G118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="H118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="I118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="J118" s="12">
+        <v>162.52000000000001</v>
+      </c>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="9">
+        <f>SUM(C118:J118)</f>
+        <v>1300.1600000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A119" s="7">
+        <v>45987</v>
+      </c>
+      <c r="B119" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C119" s="12">
+        <v>44.81</v>
+      </c>
+      <c r="D119" s="12">
+        <v>44.81</v>
+      </c>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="9">
+        <f>SUM(C119:D119)</f>
+        <v>89.62</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A120" s="7">
+        <v>45987</v>
+      </c>
+      <c r="B120" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C120" s="12">
+        <v>31.06</v>
+      </c>
+      <c r="D120" s="12">
+        <v>31.06</v>
+      </c>
+      <c r="E120" s="12">
+        <v>31.06</v>
+      </c>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="9">
+        <f>SUM(C120:E120)</f>
+        <v>93.179999999999993</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A121" s="7">
+        <v>45988</v>
+      </c>
+      <c r="B121" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="D121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="E121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="F121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="G121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="H121" s="12">
+        <v>55.71</v>
+      </c>
+      <c r="I121" s="4"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="4"/>
+      <c r="L121" s="4"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="9">
+        <f>SUM(C121:H121)</f>
+        <v>334.26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A122" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B122" s="42"/>
+      <c r="C122" s="12">
+        <f>SUM(C82:C121)</f>
+        <v>3008.7800000000007</v>
+      </c>
+      <c r="D122" s="12">
+        <f>SUM(D82:D120)</f>
+        <v>2301.6699999999996</v>
+      </c>
+      <c r="E122" s="12">
+        <f>SUM(E82:E120)</f>
+        <v>1629.1299999999999</v>
+      </c>
+      <c r="F122" s="12">
+        <f>SUM(F82:F120)</f>
+        <v>989.41</v>
+      </c>
+      <c r="G122" s="12">
+        <f>SUM(G82:G120)</f>
+        <v>823.85</v>
+      </c>
+      <c r="H122" s="12">
+        <f>SUM(H82:H120)</f>
+        <v>411.61</v>
+      </c>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
+      <c r="L122" s="4"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="12">
+        <f>SUM(C122:H122)</f>
+        <v>9164.4500000000007</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="36"/>
       <c r="B123" s="36"/>
       <c r="C123" s="36"/>
@@ -4296,18 +4522,800 @@
       <c r="N123" s="36"/>
       <c r="O123" s="36"/>
     </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A124" s="7">
+        <v>46361</v>
+      </c>
+      <c r="B124" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" s="9">
+        <v>10</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A125" s="7">
+        <v>46365</v>
+      </c>
+      <c r="B125" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C125" s="9">
+        <v>435.16</v>
+      </c>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A126" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C126" s="12">
+        <v>90</v>
+      </c>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A127" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C127" s="12">
+        <v>44.9</v>
+      </c>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="4"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="O127" s="6"/>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A128" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C128" s="12">
+        <v>64.760000000000005</v>
+      </c>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="6"/>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A129" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" s="12">
+        <v>29.99</v>
+      </c>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="6"/>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A130" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" s="12">
+        <v>31.9</v>
+      </c>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="6"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A131" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C131" s="12">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="6"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A132" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B132" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C132" s="12">
+        <v>1.99</v>
+      </c>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="6"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A133" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C133" s="12">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="6"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A134" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C134" s="12">
+        <v>66.45</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="6"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A135" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C135" s="12">
+        <v>94.37</v>
+      </c>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="6"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A136" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C136" s="12">
+        <v>118.7</v>
+      </c>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="6"/>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A137" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B137" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C137" s="12">
+        <v>50</v>
+      </c>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="6"/>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A138" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B138" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C138" s="12">
+        <v>50</v>
+      </c>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
+      <c r="L138" s="4"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="4"/>
+      <c r="O138" s="6"/>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A139" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B139" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C139" s="12">
+        <v>20.49</v>
+      </c>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="4"/>
+      <c r="L139" s="4"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="6"/>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A140" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B140" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C140" s="12">
+        <v>14.18</v>
+      </c>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="6"/>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A141" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C141" s="12">
+        <v>35.31</v>
+      </c>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="4"/>
+      <c r="L141" s="4"/>
+      <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="6"/>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A142" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C142" s="12">
+        <v>20.07</v>
+      </c>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="6"/>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A143" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C143" s="12">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="6"/>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A144" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C144" s="12">
+        <v>20.68</v>
+      </c>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="6"/>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A145" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C145" s="12">
+        <v>19.73</v>
+      </c>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="6"/>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A146" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B146" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C146" s="12">
+        <v>14.22</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="6"/>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A147" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C147" s="12">
+        <v>44.9</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="6"/>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A148" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B148" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C148" s="12">
+        <v>10</v>
+      </c>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="6"/>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A149" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C149" s="12">
+        <v>27.9</v>
+      </c>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="4"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="4"/>
+      <c r="L149" s="4"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="6"/>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A150" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C150" s="12">
+        <v>6.9</v>
+      </c>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="4"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="4"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="6"/>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A151" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B151" s="44"/>
+      <c r="C151" s="50">
+        <f>SUM(C124:C150)</f>
+        <v>1373.3000000000004</v>
+      </c>
+      <c r="D151" s="23"/>
+      <c r="E151" s="23"/>
+      <c r="F151" s="23"/>
+      <c r="G151" s="23"/>
+      <c r="H151" s="23"/>
+      <c r="I151" s="23"/>
+      <c r="J151" s="23"/>
+      <c r="K151" s="23"/>
+      <c r="L151" s="23"/>
+      <c r="M151" s="24"/>
+      <c r="N151" s="38">
+        <f>SUM(N105:N124)</f>
+        <v>0</v>
+      </c>
+      <c r="O151" s="12">
+        <f>SUM(N151)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A152" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B152" s="44"/>
+      <c r="C152" s="45">
+        <f>SUM(C151,C122)</f>
+        <v>4382.0800000000008</v>
+      </c>
+      <c r="D152" s="23"/>
+      <c r="E152" s="23"/>
+      <c r="F152" s="23"/>
+      <c r="G152" s="23"/>
+      <c r="H152" s="23"/>
+      <c r="I152" s="23"/>
+      <c r="J152" s="23"/>
+      <c r="K152" s="23"/>
+      <c r="L152" s="23"/>
+      <c r="M152" s="24"/>
+      <c r="N152" s="12">
+        <f>SUM(N101,N151)</f>
+        <v>0</v>
+      </c>
+      <c r="O152" s="25">
+        <f>SUM(N152)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A153" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B153" s="49"/>
+      <c r="D153" s="25">
+        <v>2239.48</v>
+      </c>
+      <c r="E153" s="12">
+        <v>1596.54</v>
+      </c>
+      <c r="F153" s="12">
+        <v>1010.3</v>
+      </c>
+      <c r="G153" s="12">
+        <v>844.75</v>
+      </c>
+      <c r="H153" s="12">
+        <v>432.51</v>
+      </c>
+      <c r="I153" s="12">
+        <v>262.25</v>
+      </c>
+      <c r="J153" s="12">
+        <v>262.25</v>
+      </c>
+      <c r="K153" s="4"/>
+      <c r="L153" s="4"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="40">
+        <f>SUM(C153:N153)</f>
+        <v>6648.08</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A155" s="36"/>
+      <c r="B155" s="36"/>
+      <c r="C155" s="36"/>
+      <c r="D155" s="36"/>
+      <c r="E155" s="36"/>
+      <c r="F155" s="36"/>
+      <c r="G155" s="36"/>
+      <c r="H155" s="36"/>
+      <c r="I155" s="36"/>
+      <c r="J155" s="36"/>
+      <c r="K155" s="36"/>
+      <c r="L155" s="36"/>
+      <c r="M155" s="36"/>
+      <c r="N155" s="36"/>
+      <c r="O155" s="36"/>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A156" s="36"/>
+      <c r="B156" s="36"/>
+      <c r="C156" s="36"/>
+      <c r="D156" s="36"/>
+      <c r="E156" s="36"/>
+      <c r="F156" s="36"/>
+      <c r="G156" s="36"/>
+      <c r="H156" s="36"/>
+      <c r="I156" s="36"/>
+      <c r="J156" s="36"/>
+      <c r="K156" s="36"/>
+      <c r="L156" s="36"/>
+      <c r="M156" s="36"/>
+      <c r="N156" s="36"/>
+      <c r="O156" s="36"/>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A157" s="36"/>
+      <c r="B157" s="36"/>
+      <c r="C157" s="36"/>
+      <c r="D157" s="36"/>
+      <c r="E157" s="36"/>
+      <c r="F157" s="36"/>
+      <c r="G157" s="36"/>
+      <c r="H157" s="36"/>
+      <c r="I157" s="36"/>
+      <c r="J157" s="36"/>
+      <c r="K157" s="36"/>
+      <c r="L157" s="36"/>
+      <c r="M157" s="36"/>
+      <c r="N157" s="36"/>
+      <c r="O157" s="36"/>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A158" s="36"/>
+      <c r="B158" s="36"/>
+      <c r="C158" s="36"/>
+      <c r="D158" s="36"/>
+      <c r="E158" s="36"/>
+      <c r="F158" s="36"/>
+      <c r="G158" s="36"/>
+      <c r="H158" s="36"/>
+      <c r="I158" s="36"/>
+      <c r="J158" s="36"/>
+      <c r="K158" s="36"/>
+      <c r="L158" s="36"/>
+      <c r="M158" s="36"/>
+      <c r="N158" s="36"/>
+      <c r="O158" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A112:B112"/>
+  <mergeCells count="7">
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A122:B122"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A113:B113"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="O7 O88 O95 O97" formula="1"/>
+    <ignoredError sqref="O7" formula="1"/>
     <ignoredError sqref="O12" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>

</xml_diff>

<commit_message>
Formatando data e quebra de linha
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -101,9 +101,6 @@
     <t>AMAZON BR PARC 02/04 SAO PAULO BR</t>
   </si>
   <si>
-    <t>Compra / Vencimento 10/12</t>
-  </si>
-  <si>
     <t>SHOPEE *Marav PARC 01/06 Cajamar BR</t>
   </si>
   <si>
@@ -386,9 +383,6 @@
     <t>Jose Ronierio Marinho Osasco BR</t>
   </si>
   <si>
-    <t>Compra / Vencimento 10/01</t>
-  </si>
-  <si>
     <t>09/12</t>
   </si>
   <si>
@@ -498,6 +492,12 @@
   </si>
   <si>
     <t>PGTO DEBITO CONTA 0697 000006055 200211</t>
+  </si>
+  <si>
+    <t>Transação / Vencimento 10/12</t>
+  </si>
+  <si>
+    <t>Transação / Vencimento 10/01</t>
   </si>
 </sst>
 </file>
@@ -867,6 +867,21 @@
     <xf numFmtId="165" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -884,21 +899,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1193,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:Q161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:C94"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1214,7 @@
         <v>2025</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>9</v>
@@ -1259,7 +1259,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>
       <c r="B2" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1282,7 +1282,7 @@
         <v>45971</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1305,7 +1305,7 @@
         <v>45971</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1328,7 +1328,7 @@
         <v>45972</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1351,7 +1351,7 @@
         <v>45980</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1612,7 +1612,7 @@
         <v>45964</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1635,7 +1635,7 @@
         <v>45965</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1660,7 +1660,7 @@
         <v>45965</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1685,7 +1685,7 @@
         <v>45905</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1710,7 +1710,7 @@
         <v>45905</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1740,7 +1740,7 @@
         <v>45966</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1765,7 +1765,7 @@
         <v>45966</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1790,7 +1790,7 @@
         <v>45936</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1818,7 +1818,7 @@
         <v>45876</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1850,7 +1850,7 @@
         <v>45966</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1873,7 +1873,7 @@
         <v>45966</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1896,7 +1896,7 @@
         <v>45966</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1919,7 +1919,7 @@
         <v>45966</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1942,7 +1942,7 @@
         <v>45966</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1965,7 +1965,7 @@
         <v>45966</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1988,7 +1988,7 @@
         <v>45966</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2011,7 +2011,7 @@
         <v>45966</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2034,7 +2034,7 @@
         <v>45908</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2064,7 +2064,7 @@
         <v>45878</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2096,7 +2096,7 @@
         <v>45941</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2121,7 +2121,7 @@
         <v>45942</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2149,7 +2149,7 @@
         <v>45942</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2177,7 +2177,7 @@
         <v>45701</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2221,7 +2221,7 @@
         <v>45702</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2265,7 +2265,7 @@
         <v>45915</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2295,7 +2295,7 @@
         <v>45964</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2318,7 +2318,7 @@
         <v>45964</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2341,7 +2341,7 @@
         <v>45964</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2364,7 +2364,7 @@
         <v>45964</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2387,7 +2387,7 @@
         <v>45964</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2410,7 +2410,7 @@
         <v>45858</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2444,7 +2444,7 @@
         <v>45858</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2478,7 +2478,7 @@
         <v>45923</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2503,7 +2503,7 @@
         <v>45984</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2528,7 +2528,7 @@
         <v>45984</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2553,7 +2553,7 @@
         <v>45984</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2578,7 +2578,7 @@
         <v>45954</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2603,7 +2603,7 @@
         <v>45954</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2628,7 +2628,7 @@
         <v>45954</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2653,7 +2653,7 @@
         <v>45954</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2678,7 +2678,7 @@
         <v>45987</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2728,7 +2728,7 @@
         <v>45988</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2749,10 +2749,10 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="53"/>
+      <c r="A58" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="58"/>
       <c r="C58" s="16"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2873,7 +2873,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2896,10 +2896,10 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2922,10 +2922,10 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2948,10 +2948,10 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2974,10 +2974,10 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3000,10 +3000,10 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3026,10 +3026,10 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3052,10 +3052,10 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -3104,10 +3104,10 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -3182,10 +3182,10 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="25" t="s">
         <v>90</v>
-      </c>
-      <c r="B75" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -3208,10 +3208,10 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="25" t="s">
         <v>94</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>95</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -3234,10 +3234,10 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -3260,10 +3260,10 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -3286,10 +3286,10 @@
       <c r="Q78" s="26"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A79" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" s="53"/>
+      <c r="A79" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="58"/>
       <c r="C79" s="16"/>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
@@ -3311,10 +3311,10 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A80" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B80" s="53"/>
+      <c r="A80" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="58"/>
       <c r="C80" s="16"/>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
@@ -3371,114 +3371,114 @@
       <c r="O82" s="24"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A83" s="58">
+      <c r="A83" s="52">
         <v>2026</v>
       </c>
-      <c r="B83" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="C83" s="59" t="s">
+      <c r="B83" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D83" s="59" t="s">
+      <c r="D83" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E83" s="59" t="s">
+      <c r="E83" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F83" s="59" t="s">
+      <c r="F83" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G83" s="59" t="s">
+      <c r="G83" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="H83" s="59" t="s">
+      <c r="H83" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="I83" s="59" t="s">
+      <c r="I83" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="J83" s="59" t="s">
+      <c r="J83" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K83" s="59" t="s">
+      <c r="K83" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="L83" s="59" t="s">
+      <c r="L83" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="M83" s="59" t="s">
+      <c r="M83" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="N83" s="59" t="s">
+      <c r="N83" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="O83" s="60" t="s">
+      <c r="O83" s="54" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="61"/>
-      <c r="B84" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="59"/>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
-      <c r="H84" s="59"/>
-      <c r="I84" s="59"/>
-      <c r="J84" s="59"/>
-      <c r="K84" s="59"/>
-      <c r="L84" s="59"/>
-      <c r="M84" s="59"/>
+      <c r="A84" s="55"/>
+      <c r="B84" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="C84" s="53"/>
+      <c r="D84" s="53"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="53"/>
+      <c r="G84" s="53"/>
+      <c r="H84" s="53"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="53"/>
+      <c r="M84" s="53"/>
       <c r="N84" s="48">
         <v>3906.89</v>
       </c>
       <c r="O84" s="46"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A85" s="62">
+      <c r="A85" s="56">
         <v>46358</v>
       </c>
-      <c r="B85" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" s="59"/>
-      <c r="D85" s="59"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="59"/>
-      <c r="G85" s="59"/>
-      <c r="H85" s="59"/>
-      <c r="I85" s="59"/>
-      <c r="J85" s="59"/>
-      <c r="K85" s="59"/>
-      <c r="L85" s="59"/>
-      <c r="M85" s="59"/>
+      <c r="B85" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="53"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="53"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="53"/>
+      <c r="M85" s="53"/>
       <c r="N85" s="48">
         <v>-45.5</v>
       </c>
       <c r="O85" s="46"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A86" s="62">
+      <c r="A86" s="56">
         <v>46001</v>
       </c>
-      <c r="B86" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="C86" s="59"/>
-      <c r="D86" s="59"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="59"/>
-      <c r="G86" s="59"/>
-      <c r="H86" s="59"/>
-      <c r="I86" s="59"/>
-      <c r="J86" s="59"/>
-      <c r="K86" s="59"/>
-      <c r="L86" s="59"/>
-      <c r="M86" s="59"/>
+      <c r="B86" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C86" s="53"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="53"/>
+      <c r="G86" s="53"/>
+      <c r="H86" s="53"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="53"/>
+      <c r="M86" s="53"/>
       <c r="N86" s="48">
         <v>-3906.89</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>45834</v>
       </c>
       <c r="B87" s="51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87" s="50">
         <v>54.5</v>
@@ -3512,10 +3512,10 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B88" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C88" s="30">
         <v>34.090000000000003</v>
@@ -3538,10 +3538,10 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C89" s="30">
         <v>165.26</v>
@@ -3566,10 +3566,10 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B90" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C90" s="30">
         <v>29.58</v>
@@ -3597,7 +3597,7 @@
         <v>45959</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91" s="7">
         <v>22.86</v>
@@ -3626,10 +3626,10 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B92" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C92" s="33">
         <v>21.63</v>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93" s="7">
         <v>52.81</v>
@@ -3689,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94" s="7">
         <v>29.8</v>
@@ -3721,7 +3721,7 @@
         <v>45930</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C95" s="7">
         <v>32.93</v>
@@ -3749,7 +3749,7 @@
         <v>3</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C96" s="7">
         <v>58.09</v>
@@ -3779,7 +3779,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C97" s="7">
         <v>183.99</v>
@@ -3807,7 +3807,7 @@
         <v>45965</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C98" s="9">
         <v>75.040000000000006</v>
@@ -3835,7 +3835,7 @@
         <v>45965</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C99" s="9">
         <v>121.25</v>
@@ -3869,7 +3869,7 @@
         <v>45905</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C100" s="9">
         <v>71.989999999999995</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B101" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C101" s="33">
         <v>114.59</v>
@@ -3931,7 +3931,7 @@
         <v>45936</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C102" s="9">
         <v>210.89</v>
@@ -3957,7 +3957,7 @@
         <v>45876</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C103" s="9">
         <v>83.88</v>
@@ -3983,7 +3983,7 @@
         <v>45908</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C104" s="9">
         <v>29.73</v>
@@ -4009,7 +4009,7 @@
         <v>45878</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C105" s="9">
         <v>78.55</v>
@@ -4036,10 +4036,10 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B106" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C106" s="33">
         <v>111.2</v>
@@ -4066,10 +4066,10 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B107" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C107" s="33">
         <v>203.32</v>
@@ -4099,7 +4099,7 @@
         <v>45942</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C108" s="9">
         <v>62.43</v>
@@ -4125,7 +4125,7 @@
         <v>45942</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C109" s="9">
         <v>20.47</v>
@@ -4150,10 +4150,10 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B110" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C110" s="33">
         <v>27.89</v>
@@ -4181,7 +4181,7 @@
         <v>45858</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C111" s="9">
         <v>52.74</v>
@@ -4207,7 +4207,7 @@
         <v>45923</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C112" s="9">
         <v>290.99</v>
@@ -4241,7 +4241,7 @@
         <v>45984</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C113" s="9">
         <v>52.25</v>
@@ -4269,7 +4269,7 @@
         <v>45984</v>
       </c>
       <c r="B114" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C114" s="9">
         <v>37.630000000000003</v>
@@ -4301,7 +4301,7 @@
         <v>45984</v>
       </c>
       <c r="B115" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C115" s="9">
         <v>75.260000000000005</v>
@@ -4330,10 +4330,10 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B116" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C116" s="33">
         <v>83.06</v>
@@ -4363,7 +4363,7 @@
         <v>45954</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C117" s="9">
         <v>96.66</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B118" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C118" s="33">
         <v>34.770000000000003</v>
@@ -4433,7 +4433,7 @@
         <v>45954</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C119" s="9">
         <v>40.32</v>
@@ -4461,7 +4461,7 @@
         <v>45954</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120" s="9">
         <v>99.73</v>
@@ -4501,7 +4501,7 @@
         <v>45954</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C121" s="9">
         <v>162.52000000000001</v>
@@ -4541,7 +4541,7 @@
         <v>45987</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C122" s="9">
         <v>44.79</v>
@@ -4569,7 +4569,7 @@
         <v>45987</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C123" s="9">
         <v>31.06</v>
@@ -4599,7 +4599,7 @@
         <v>45988</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C124" s="9">
         <v>55.71</v>
@@ -4631,10 +4631,10 @@
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A125" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="B125" s="57"/>
+      <c r="A125" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B125" s="62"/>
       <c r="C125" s="9">
         <f>SUM(C85:C124)</f>
         <v>3054.2600000000007</v>
@@ -4710,7 +4710,7 @@
         <v>46361</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C127" s="7">
         <v>10</v>
@@ -4733,7 +4733,7 @@
         <v>46365</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C128" s="7">
         <v>435.16</v>
@@ -4753,10 +4753,10 @@
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C129" s="36">
         <v>90</v>
@@ -4800,10 +4800,10 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C130" s="9">
         <v>44.9</v>
@@ -4823,10 +4823,10 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C131" s="9">
         <v>64.760000000000005</v>
@@ -4846,10 +4846,10 @@
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C132" s="9">
         <v>29.99</v>
@@ -4869,10 +4869,10 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C133" s="9">
         <v>31.9</v>
@@ -4892,10 +4892,10 @@
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C134" s="9">
         <v>16.989999999999998</v>
@@ -4915,10 +4915,10 @@
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C135" s="9">
         <v>1.99</v>
@@ -4938,10 +4938,10 @@
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C136" s="9">
         <v>16.899999999999999</v>
@@ -4961,10 +4961,10 @@
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C137" s="9">
         <v>66.45</v>
@@ -4984,10 +4984,10 @@
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C138" s="9">
         <v>94.37</v>
@@ -5007,10 +5007,10 @@
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C139" s="9">
         <v>118.7</v>
@@ -5030,10 +5030,10 @@
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C140" s="9">
         <v>50</v>
@@ -5053,10 +5053,10 @@
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C141" s="9">
         <v>50</v>
@@ -5076,10 +5076,10 @@
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C142" s="9">
         <v>20.49</v>
@@ -5099,10 +5099,10 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C143" s="9">
         <v>14.18</v>
@@ -5122,10 +5122,10 @@
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C144" s="9">
         <v>35.31</v>
@@ -5145,10 +5145,10 @@
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C145" s="9">
         <v>20.07</v>
@@ -5168,10 +5168,10 @@
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C146" s="9">
         <v>16.809999999999999</v>
@@ -5191,10 +5191,10 @@
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C147" s="9">
         <v>20.68</v>
@@ -5214,10 +5214,10 @@
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C148" s="9">
         <v>19.73</v>
@@ -5237,10 +5237,10 @@
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C149" s="9">
         <v>14.22</v>
@@ -5260,10 +5260,10 @@
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C150" s="9">
         <v>44.9</v>
@@ -5283,10 +5283,10 @@
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C151" s="9">
         <v>10</v>
@@ -5306,10 +5306,10 @@
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C152" s="9">
         <v>27.9</v>
@@ -5329,10 +5329,10 @@
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B153" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="C153" s="9">
         <v>6.9</v>
@@ -5351,10 +5351,10 @@
       <c r="O153" s="4"/>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A154" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="B154" s="53"/>
+      <c r="A154" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B154" s="58"/>
       <c r="C154" s="36">
         <f>SUM(C127:C153)</f>
         <v>1373.3000000000004</v>
@@ -5409,10 +5409,10 @@
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A155" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B155" s="53"/>
+      <c r="A155" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B155" s="58"/>
       <c r="C155" s="37">
         <f>SUM(C154,C125)</f>
         <v>4427.5600000000013</v>
@@ -5467,10 +5467,10 @@
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A156" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="B156" s="55"/>
+      <c r="A156" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B156" s="60"/>
       <c r="C156" s="19">
         <v>4382.0600000000004</v>
       </c>

</xml_diff>

<commit_message>
restaurando arquivos e formatando largura de coluna
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\projeto_planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\projeto_planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -1193,23 +1193,22 @@
   </sheetPr>
   <dimension ref="A1:Q161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P159" sqref="P159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" customWidth="1"/>
-    <col min="3" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="3" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="47">
         <v>2025</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
       <c r="B2" s="23" t="s">
         <v>153</v>
@@ -1277,7 +1276,7 @@
       </c>
       <c r="O2" s="34"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>45971</v>
       </c>
@@ -1300,7 +1299,7 @@
       </c>
       <c r="O3" s="34"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>45971</v>
       </c>
@@ -1323,7 +1322,7 @@
       </c>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>45972</v>
       </c>
@@ -1346,7 +1345,7 @@
       </c>
       <c r="O5" s="34"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>45980</v>
       </c>
@@ -1369,7 +1368,7 @@
       </c>
       <c r="O6" s="34"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>45834</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>45959</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>22.86</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>45930</v>
       </c>
@@ -1457,7 +1456,7 @@
         <v>65.86</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>52.81</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1508,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>174.3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>1287.93</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>45964</v>
       </c>
@@ -1630,7 +1629,7 @@
       </c>
       <c r="O15" s="42"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>45965</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>75.040000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>45965</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>121.26</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>45905</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>55.74</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>45905</v>
       </c>
@@ -1735,7 +1734,7 @@
         <v>215.96999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>45966</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>729.61</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>45966</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>723.79</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>45936</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>421.78</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>45876</v>
       </c>
@@ -1845,7 +1844,7 @@
         <v>335.52</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>45966</v>
       </c>
@@ -1868,7 +1867,7 @@
       </c>
       <c r="O24" s="42"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>45966</v>
       </c>
@@ -1891,7 +1890,7 @@
       </c>
       <c r="O25" s="42"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>45966</v>
       </c>
@@ -1914,7 +1913,7 @@
       </c>
       <c r="O26" s="42"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>45966</v>
       </c>
@@ -1937,7 +1936,7 @@
       </c>
       <c r="O27" s="42"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>45966</v>
       </c>
@@ -1960,7 +1959,7 @@
       </c>
       <c r="O28" s="42"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>45966</v>
       </c>
@@ -1983,7 +1982,7 @@
       </c>
       <c r="O29" s="42"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>45966</v>
       </c>
@@ -2006,7 +2005,7 @@
       </c>
       <c r="O30" s="42"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>45966</v>
       </c>
@@ -2029,7 +2028,7 @@
       </c>
       <c r="O31" s="42"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>45908</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>89.19</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>45878</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>314.2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>45941</v>
       </c>
@@ -2116,7 +2115,7 @@
         <v>119.71</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>45942</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>124.86</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>45942</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>40.94</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>45701</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>1032.3999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>45702</v>
       </c>
@@ -2260,7 +2259,7 @@
         <v>1116.5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>45915</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>391.26</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>45964</v>
       </c>
@@ -2313,7 +2312,7 @@
       </c>
       <c r="O40" s="42"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>45964</v>
       </c>
@@ -2336,7 +2335,7 @@
       </c>
       <c r="O41" s="42"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>45964</v>
       </c>
@@ -2359,7 +2358,7 @@
       </c>
       <c r="O42" s="42"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>45964</v>
       </c>
@@ -2382,7 +2381,7 @@
       </c>
       <c r="O43" s="42"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>45964</v>
       </c>
@@ -2405,7 +2404,7 @@
       </c>
       <c r="O44" s="42"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>45858</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>299.95</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45858</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>263.7</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>45923</v>
       </c>
@@ -2498,7 +2497,7 @@
         <v>290.99</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>45984</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>52.27</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>45984</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>75.28</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>45984</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>37.64</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>45954</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>96.66</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>45954</v>
       </c>
@@ -2623,7 +2622,7 @@
         <v>40.32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>45954</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>99.73</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>45954</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>162.52000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>45987</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>44.81</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>45987</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>31.06</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>45988</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>55.74</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="57" t="s">
         <v>85</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>2893.7400000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="38"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -2790,7 +2789,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="40"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>65</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>0</v>
       </c>
@@ -2842,7 +2841,7 @@
         <v>136.86000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>65</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>45.61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>3</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>66</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>67</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>67</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>67</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>68</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>37.950000000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>68</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>99.34</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>68</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>42.28</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>69</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>71.81</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>70</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>71</v>
       </c>
@@ -3154,7 +3153,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>72</v>
       </c>
@@ -3180,7 +3179,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>89</v>
       </c>
@@ -3206,7 +3205,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>93</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
         <v>67</v>
       </c>
@@ -3258,7 +3257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>92</v>
       </c>
@@ -3285,7 +3284,7 @@
       </c>
       <c r="Q78" s="26"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="57" t="s">
         <v>86</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>1013.1499999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="57" t="s">
         <v>87</v>
       </c>
@@ -3336,7 +3335,7 @@
       </c>
       <c r="Q80" s="26"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="24"/>
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
@@ -3353,7 +3352,7 @@
       <c r="N81" s="24"/>
       <c r="O81" s="24"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="24"/>
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
@@ -3370,7 +3369,7 @@
       <c r="N82" s="24"/>
       <c r="O82" s="24"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="52">
         <v>2026</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="55"/>
       <c r="B84" s="53" t="s">
         <v>153</v>
@@ -3438,7 +3437,7 @@
       </c>
       <c r="O84" s="46"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="56">
         <v>46358</v>
       </c>
@@ -3461,7 +3460,7 @@
       </c>
       <c r="O85" s="46"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="56">
         <v>46001</v>
       </c>
@@ -3484,7 +3483,7 @@
       </c>
       <c r="O86" s="46"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
         <v>45834</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>54.5</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
         <v>140</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>34.090000000000003</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
         <v>141</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>330.52</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
         <v>141</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>59.16</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>45959</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>91.44</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="s">
         <v>143</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>64.89</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>0</v>
       </c>
@@ -3684,7 +3683,7 @@
         <v>158.43</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>0</v>
       </c>
@@ -3716,7 +3715,7 @@
         <v>119.2</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>45930</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>65.86</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>3</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>174.27</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +3801,7 @@
         <v>367.98</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>45965</v>
       </c>
@@ -3830,7 +3829,7 @@
         <v>150.08000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>45965</v>
       </c>
@@ -3864,7 +3863,7 @@
         <v>606.25</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>45905</v>
       </c>
@@ -3890,7 +3889,7 @@
         <v>71.989999999999995</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="31" t="s">
         <v>145</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>114.59</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>45936</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>210.89</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>45876</v>
       </c>
@@ -3978,7 +3977,7 @@
         <v>83.88</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>45908</v>
       </c>
@@ -4004,7 +4003,7 @@
         <v>29.73</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>45878</v>
       </c>
@@ -4034,7 +4033,7 @@
         <v>235.64999999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>146</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>333.6</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>135</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>609.96</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>45942</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>62.43</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>45942</v>
       </c>
@@ -4148,7 +4147,7 @@
         <v>40.94</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="31" t="s">
         <v>149</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>55.78</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>45858</v>
       </c>
@@ -4202,7 +4201,7 @@
         <v>52.74</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>45923</v>
       </c>
@@ -4236,7 +4235,7 @@
         <v>1454.95</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>45984</v>
       </c>
@@ -4264,7 +4263,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>45984</v>
       </c>
@@ -4296,7 +4295,7 @@
         <v>150.55000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>45984</v>
       </c>
@@ -4328,7 +4327,7 @@
         <v>301.04000000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="31" t="s">
         <v>151</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>249.18</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>45954</v>
       </c>
@@ -4384,7 +4383,7 @@
         <v>96.66</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="31" t="s">
         <v>151</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>347.7</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>45954</v>
       </c>
@@ -4456,7 +4455,7 @@
         <v>80.64</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>45954</v>
       </c>
@@ -4496,7 +4495,7 @@
         <v>797.84</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>45954</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>1300.1600000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>45987</v>
       </c>
@@ -4564,7 +4563,7 @@
         <v>89.6</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>45987</v>
       </c>
@@ -4594,7 +4593,7 @@
         <v>93.179999999999993</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>45988</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>334.26</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="61" t="s">
         <v>85</v>
       </c>
@@ -4688,7 +4687,7 @@
         <v>9488.48</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="38"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -4705,7 +4704,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="40"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>46361</v>
       </c>
@@ -4728,7 +4727,7 @@
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>46365</v>
       </c>
@@ -4751,7 +4750,7 @@
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
         <v>66</v>
       </c>
@@ -4798,7 +4797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>121</v>
       </c>
@@ -4821,7 +4820,7 @@
       <c r="N130" s="2"/>
       <c r="O130" s="4"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>123</v>
       </c>
@@ -4844,7 +4843,7 @@
       <c r="N131" s="2"/>
       <c r="O131" s="4"/>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>125</v>
       </c>
@@ -4867,7 +4866,7 @@
       <c r="N132" s="2"/>
       <c r="O132" s="4"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>127</v>
       </c>
@@ -4890,7 +4889,7 @@
       <c r="N133" s="2"/>
       <c r="O133" s="4"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>127</v>
       </c>
@@ -4913,7 +4912,7 @@
       <c r="N134" s="2"/>
       <c r="O134" s="4"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>125</v>
       </c>
@@ -4936,7 +4935,7 @@
       <c r="N135" s="2"/>
       <c r="O135" s="4"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>128</v>
       </c>
@@ -4959,7 +4958,7 @@
       <c r="N136" s="2"/>
       <c r="O136" s="4"/>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>125</v>
       </c>
@@ -4982,7 +4981,7 @@
       <c r="N137" s="2"/>
       <c r="O137" s="4"/>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
         <v>123</v>
       </c>
@@ -5005,7 +5004,7 @@
       <c r="N138" s="2"/>
       <c r="O138" s="4"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>130</v>
       </c>
@@ -5028,7 +5027,7 @@
       <c r="N139" s="2"/>
       <c r="O139" s="4"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>131</v>
       </c>
@@ -5051,7 +5050,7 @@
       <c r="N140" s="2"/>
       <c r="O140" s="4"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
         <v>133</v>
       </c>
@@ -5074,7 +5073,7 @@
       <c r="N141" s="2"/>
       <c r="O141" s="4"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>119</v>
       </c>
@@ -5097,7 +5096,7 @@
       <c r="N142" s="2"/>
       <c r="O142" s="4"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>119</v>
       </c>
@@ -5120,7 +5119,7 @@
       <c r="N143" s="2"/>
       <c r="O143" s="4"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
         <v>135</v>
       </c>
@@ -5143,7 +5142,7 @@
       <c r="N144" s="2"/>
       <c r="O144" s="4"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
         <v>135</v>
       </c>
@@ -5166,7 +5165,7 @@
       <c r="N145" s="2"/>
       <c r="O145" s="4"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>125</v>
       </c>
@@ -5189,7 +5188,7 @@
       <c r="N146" s="2"/>
       <c r="O146" s="4"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
         <v>125</v>
       </c>
@@ -5212,7 +5211,7 @@
       <c r="N147" s="2"/>
       <c r="O147" s="4"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
         <v>128</v>
       </c>
@@ -5235,7 +5234,7 @@
       <c r="N148" s="2"/>
       <c r="O148" s="4"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>127</v>
       </c>
@@ -5258,7 +5257,7 @@
       <c r="N149" s="2"/>
       <c r="O149" s="4"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>121</v>
       </c>
@@ -5281,7 +5280,7 @@
       <c r="N150" s="2"/>
       <c r="O150" s="4"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>131</v>
       </c>
@@ -5304,7 +5303,7 @@
       <c r="N151" s="2"/>
       <c r="O151" s="4"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>137</v>
       </c>
@@ -5327,7 +5326,7 @@
       <c r="N152" s="2"/>
       <c r="O152" s="4"/>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>137</v>
       </c>
@@ -5350,7 +5349,7 @@
       <c r="N153" s="2"/>
       <c r="O153" s="4"/>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="57" t="s">
         <v>86</v>
       </c>
@@ -5408,7 +5407,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="57" t="s">
         <v>87</v>
       </c>
@@ -5466,7 +5465,7 @@
         <v>12515.360000000002</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="59" t="s">
         <v>116</v>
       </c>
@@ -5504,7 +5503,7 @@
         <v>11030.140000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="24"/>
       <c r="B158" s="24"/>
       <c r="C158" s="24"/>
@@ -5521,7 +5520,7 @@
       <c r="N158" s="24"/>
       <c r="O158" s="24"/>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="24"/>
       <c r="B159" s="24"/>
       <c r="C159" s="24"/>
@@ -5538,7 +5537,7 @@
       <c r="N159" s="24"/>
       <c r="O159" s="24"/>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="24"/>
       <c r="B160" s="24"/>
       <c r="C160" s="24"/>
@@ -5555,7 +5554,7 @@
       <c r="N160" s="24"/>
       <c r="O160" s="24"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="24"/>
       <c r="B161" s="24"/>
       <c r="C161" s="24"/>

</xml_diff>